<commit_message>
fixed mistake in fortrængning ved alle biogas beregninger.
</commit_message>
<xml_diff>
--- a/output/emis_table_DyrSamlet_KVIK.xlsx
+++ b/output/emis_table_DyrSamlet_KVIK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au277187_uni_au_dk/Documents/Documents/GitHub/AU-BCE-EE/Dalby-2025-KVIK/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_CCE2F2250099EBE3A88720FA5F3D0127CA9C59BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{980234F4-0E1A-4F8A-9B57-98C950A880EF}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_CDE2F22500996BD198272FFA5F3D0111EA596A3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB900B0E-A937-4C3D-B57E-0B5202A6487D}"/>
   <bookViews>
-    <workbookView xWindow="-29325" yWindow="4410" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -434,13 +434,21 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,10 +491,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1316.4535958352501</v>
+        <v>1036.72002250176</v>
       </c>
       <c r="D2">
-        <v>105.328695313418</v>
+        <v>82.9459786893716</v>
       </c>
       <c r="E2">
         <v>2.2151383863830199</v>
@@ -515,10 +523,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1034.6095200239299</v>
+        <v>708.75764551432405</v>
       </c>
       <c r="D3">
-        <v>96.277675017099597</v>
+        <v>65.954871804325506</v>
       </c>
       <c r="E3">
         <v>0.79703064504316601</v>
@@ -759,10 +767,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>1419.5877515637501</v>
+        <v>1134.1193080038599</v>
       </c>
       <c r="D11">
-        <v>116.503043114663</v>
+        <v>93.074749339300894</v>
       </c>
       <c r="E11">
         <v>1.8572919817842699</v>
@@ -1015,10 +1023,10 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>1512.3636032244699</v>
+        <v>1226.5554600062001</v>
       </c>
       <c r="D19">
-        <v>136.11705081691301</v>
+        <v>110.482338950433</v>
       </c>
       <c r="E19">
         <v>1.21000530358639</v>
@@ -1047,10 +1055,10 @@
         <v>12</v>
       </c>
       <c r="C20">
-        <v>630.53837982288098</v>
+        <v>469.68380389112099</v>
       </c>
       <c r="D20">
-        <v>125.14726347858</v>
+        <v>93.221355968363</v>
       </c>
       <c r="E20">
         <v>0.151039211198773</v>

</xml_diff>

<commit_message>
add some columns for KVIK table in output files
</commit_message>
<xml_diff>
--- a/output/emis_table_DyrSamlet_KVIK.xlsx
+++ b/output/emis_table_DyrSamlet_KVIK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Scenarie</t>
   </si>
@@ -24,6 +24,15 @@
   </si>
   <si>
     <t xml:space="preserve">mean_reduktion_totCO2_eq_tot_m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_reduktion_CH4_CO2_eq_tot_m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_reduktion_N2O_CO2_eq_tot_m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_reduktion_strøm_CO2_eq_tot_m3</t>
   </si>
   <si>
     <t xml:space="preserve">CH4_dyr_stald</t>
@@ -452,13 +461,22 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>1036.72002250176</v>
@@ -467,30 +485,39 @@
         <v>82.9459786893716</v>
       </c>
       <c r="E2" t="n">
+        <v>73.7978673334683</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9.14811135590323</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>2.21513838638302</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>0.132125130982424</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>2.34726351736545</v>
       </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
         <v>0.0154179032490679</v>
       </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>20</v>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>22.3827166240467</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="n">
         <v>708.757645514324</v>
@@ -499,30 +526,39 @@
         <v>65.9548718043255</v>
       </c>
       <c r="E3" t="n">
+        <v>55.7493691804035</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10.205502623922</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.797030645043166</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>0.335943055072568</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>1.13297370011573</v>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>0.0137483588446741</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>31</v>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>30.3228032127741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
         <v>826.918946721637</v>
@@ -531,30 +567,39 @@
         <v>52.9206439812139</v>
       </c>
       <c r="E4" t="n">
+        <v>52.9206439812139</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>2.03214149184662</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
         <v>1.0607371452422</v>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>3.09287863708882</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>0.0499390781770046</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>672.078377847682</v>
@@ -563,30 +608,39 @@
         <v>43.1537099295105</v>
       </c>
       <c r="E5" t="n">
+        <v>43.1537099295105</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.715891464956563</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
         <v>0.866927208405346</v>
       </c>
-      <c r="G5" t="n">
+      <c r="J5" t="n">
         <v>1.58281867336191</v>
       </c>
-      <c r="H5" t="n">
+      <c r="K5" t="n">
         <v>0.0522596895009837</v>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
       <c r="C6" t="n">
         <v>1513.32756807835</v>
@@ -595,30 +649,39 @@
         <v>99.1811026667696</v>
       </c>
       <c r="E6" t="n">
+        <v>97.7007238992046</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.48037876756502</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.609642447553987</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
         <v>0.883947621035164</v>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
         <v>1.49359006858915</v>
       </c>
-      <c r="H6" t="n">
+      <c r="K6" t="n">
         <v>0.0443527432050612</v>
       </c>
-      <c r="I6" t="n">
+      <c r="L6" t="n">
         <v>2.27325899081084</v>
       </c>
-      <c r="J6" t="n">
+      <c r="M6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
         <v>471.885690956768</v>
@@ -627,150 +690,195 @@
         <v>68.8796410403978</v>
       </c>
       <c r="E7" t="n">
+        <v>68.4377502242438</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.441890816153944</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.435910083451272</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
         <v>0.611606501613683</v>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
         <v>1.04751658506496</v>
       </c>
-      <c r="H7" t="n">
+      <c r="K7" t="n">
         <v>0.0492999250450266</v>
       </c>
-      <c r="I7" t="n">
+      <c r="L7" t="n">
         <v>6.1779636</v>
       </c>
-      <c r="J7" t="n">
+      <c r="M7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>2.04480125560603</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
         <v>2.93810038081185</v>
       </c>
-      <c r="G8" t="n">
+      <c r="J8" t="n">
         <v>4.98290163641789</v>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>0.0499390781770046</v>
       </c>
-      <c r="I8"/>
-      <c r="J8" t="n">
+      <c r="L8"/>
+      <c r="M8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.715891464956563</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>2.40813113445929</v>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>3.12402259941586</v>
       </c>
-      <c r="H9" t="n">
+      <c r="K9" t="n">
         <v>0.0522596895009837</v>
       </c>
-      <c r="I9"/>
-      <c r="J9" t="n">
+      <c r="L9"/>
+      <c r="M9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>50.5947650499816</v>
+        <v>72.1844592942545</v>
       </c>
       <c r="D10" t="n">
         <v>3.46056681553253</v>
       </c>
       <c r="E10" t="n">
+        <v>3.17867837967558</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.76235567567264</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1.48046723981568</v>
+      </c>
+      <c r="H10" t="n">
         <v>1.70807097571848</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>3.16130643285385</v>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
         <v>4.86937740857233</v>
       </c>
-      <c r="H10" t="n">
+      <c r="K10" t="n">
         <v>0.0432886794008814</v>
       </c>
-      <c r="I10" t="n">
+      <c r="L10" t="n">
         <v>6.23156523170345</v>
       </c>
-      <c r="J10" t="n">
+      <c r="M10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>1134.11930800386</v>
+        <v>1152.12848461255</v>
       </c>
       <c r="D11" t="n">
         <v>93.0747493393009</v>
       </c>
       <c r="E11" t="n">
+        <v>83.6447495475407</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10.9104670315759</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-1.48046723981568</v>
+      </c>
+      <c r="H11" t="n">
         <v>1.85729198178427</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
         <v>0.13829717079288</v>
       </c>
-      <c r="G11" t="n">
+      <c r="J11" t="n">
         <v>1.99558915257715</v>
       </c>
-      <c r="H11" t="n">
+      <c r="K11" t="n">
         <v>0.00876750447294472</v>
       </c>
-      <c r="I11" t="n">
+      <c r="L11" t="n">
         <v>22</v>
       </c>
-      <c r="J11" t="n">
+      <c r="M11" t="n">
         <v>23.4282937753622</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
         <v>907.141862668262</v>
@@ -779,30 +887,39 @@
         <v>58.054959410314</v>
       </c>
       <c r="E12" t="n">
+        <v>57.8707506590108</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.184208751303223</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>2.03214149184662</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
         <v>0.883947621035164</v>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
         <v>2.91608911288179</v>
       </c>
-      <c r="H12" t="n">
+      <c r="K12" t="n">
         <v>0.0492439508135962</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
         <v>738.599963224235</v>
@@ -811,30 +928,39 @@
         <v>47.4250171073789</v>
       </c>
       <c r="E13" t="n">
+        <v>47.1993702354021</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.225646871976753</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.715891464956563</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
         <v>0.722439340337788</v>
       </c>
-      <c r="G13" t="n">
+      <c r="J13" t="n">
         <v>1.43833080529435</v>
       </c>
-      <c r="H13" t="n">
+      <c r="K13" t="n">
         <v>0.0514081918708827</v>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
         <v>174.762794381444</v>
@@ -843,30 +969,39 @@
         <v>17.0032442509388</v>
       </c>
       <c r="E14" t="n">
+        <v>17.0032442509388</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.181506082574149</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
         <v>4.24935379527866</v>
       </c>
-      <c r="G14" t="n">
+      <c r="J14" t="n">
         <v>4.43085987785281</v>
       </c>
-      <c r="H14" t="n">
+      <c r="K14" t="n">
         <v>0.0523585621536815</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
         <v>9.31552116376757</v>
       </c>
-      <c r="J14" t="n">
+      <c r="M14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
         <v>517.528357405148</v>
@@ -875,30 +1010,39 @@
         <v>33.1202172700263</v>
       </c>
       <c r="E15" t="n">
+        <v>33.1202172700263</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
         <v>2.03214149184662</v>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
         <v>1.76789524207033</v>
       </c>
-      <c r="G15" t="n">
+      <c r="J15" t="n">
         <v>3.80003673391695</v>
       </c>
-      <c r="H15" t="n">
+      <c r="K15" t="n">
         <v>0.0499390781770046</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
         <v>420.0489861548</v>
@@ -907,30 +1051,39 @@
         <v>26.971068705944</v>
       </c>
       <c r="E16" t="n">
+        <v>26.971068705944</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
         <v>0.715891464956563</v>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
         <v>1.44487868067558</v>
       </c>
-      <c r="G16" t="n">
+      <c r="J16" t="n">
         <v>2.16077014563214</v>
       </c>
-      <c r="H16" t="n">
+      <c r="K16" t="n">
         <v>0.0522596895009837</v>
       </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C17" t="n">
         <v>128.927468815046</v>
@@ -939,30 +1092,39 @@
         <v>9.78245116315752</v>
       </c>
       <c r="E17" t="n">
+        <v>9.78245116315753</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.999442862143887</v>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
         <v>3.63193618775267</v>
       </c>
-      <c r="G17" t="n">
+      <c r="J17" t="n">
         <v>4.63137904989656</v>
       </c>
-      <c r="H17" t="n">
+      <c r="K17" t="n">
         <v>0.0497962344548826</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
         <v>6.99851144309235</v>
       </c>
-      <c r="J17" t="n">
+      <c r="M17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C18" t="n">
         <v>137.484122260649</v>
@@ -971,30 +1133,39 @@
         <v>18.8283155063144</v>
       </c>
       <c r="E18" t="n">
+        <v>19.473049581511</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.644734075196555</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.0588039491176154</v>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
         <v>2.73745194461637</v>
       </c>
-      <c r="G18" t="n">
+      <c r="J18" t="n">
         <v>2.79625589373399</v>
       </c>
-      <c r="H18" t="n">
+      <c r="K18" t="n">
         <v>0.0534003963331417</v>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C19" t="n">
         <v>1226.5554600062</v>
@@ -1003,30 +1174,39 @@
         <v>110.482338950433</v>
       </c>
       <c r="E19" t="n">
+        <v>101.343909794764</v>
+      </c>
+      <c r="F19" t="n">
+        <v>9.13842915566874</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
         <v>1.21000530358639</v>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
         <v>0.15132165232421</v>
       </c>
-      <c r="G19" t="n">
+      <c r="J19" t="n">
         <v>1.3613269559106</v>
       </c>
-      <c r="H19" t="n">
+      <c r="K19" t="n">
         <v>0.0153115961316043</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
         <v>24.9178856657503</v>
       </c>
-      <c r="J19" t="n">
+      <c r="M19" t="n">
         <v>25.6347118664796</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20" t="n">
         <v>469.683803891121</v>
@@ -1035,30 +1215,39 @@
         <v>93.221355968363</v>
       </c>
       <c r="E20" t="n">
+        <v>83.6605874196375</v>
+      </c>
+      <c r="F20" t="n">
+        <v>9.56076854872548</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
         <v>0.151039211198773</v>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
         <v>0.352804616887837</v>
       </c>
-      <c r="G20" t="n">
+      <c r="J20" t="n">
         <v>0.50384382808661</v>
       </c>
-      <c r="H20" t="n">
+      <c r="K20" t="n">
         <v>0.0148890656768321</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
         <v>31</v>
       </c>
-      <c r="J20" t="n">
+      <c r="M20" t="n">
         <v>31.9259075102166</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C21" t="n">
         <v>1051.67780717244</v>
@@ -1067,30 +1256,39 @@
         <v>75.6917527052212</v>
       </c>
       <c r="E21" t="n">
+        <v>75.5409009168016</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.150851788419652</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>0.971071249616833</v>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
         <v>1.31394106834385</v>
       </c>
-      <c r="G21" t="n">
+      <c r="J21" t="n">
         <v>2.28501231796069</v>
       </c>
-      <c r="H21" t="n">
+      <c r="K21" t="n">
         <v>0.0493698261452324</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
         <v>6.91275271931642</v>
       </c>
-      <c r="J21" t="n">
+      <c r="M21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C22" t="n">
         <v>494.613111396743</v>
@@ -1099,30 +1297,39 @@
         <v>67.7367797954313</v>
       </c>
       <c r="E22" t="n">
+        <v>68.3815138706278</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-0.644734075196555</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
         <v>0.0651955322211558</v>
       </c>
-      <c r="F22" t="n">
+      <c r="I22" t="n">
         <v>0.98432949404437</v>
       </c>
-      <c r="G22" t="n">
+      <c r="J22" t="n">
         <v>1.04952502626553</v>
       </c>
-      <c r="H22" t="n">
+      <c r="K22" t="n">
         <v>0.0534003963331417</v>
       </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C23" t="n">
         <v>1124.87066875679</v>
@@ -1131,30 +1338,39 @@
         <v>81.0438374359387</v>
       </c>
       <c r="E23" t="n">
+        <v>80.8596286846354</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.184208751303223</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
         <v>1.00731407275454</v>
       </c>
-      <c r="F23" t="n">
+      <c r="I23" t="n">
         <v>1.08774368206922</v>
       </c>
-      <c r="G23" t="n">
+      <c r="J23" t="n">
         <v>2.09505775482376</v>
       </c>
-      <c r="H23" t="n">
+      <c r="K23" t="n">
         <v>0.0492439508135962</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
         <v>6.91275271931642</v>
       </c>
-      <c r="J23" t="n">
+      <c r="M23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C24" t="n">
         <v>529.779752588641</v>
@@ -1163,30 +1379,39 @@
         <v>72.5528167658905</v>
       </c>
       <c r="E24" t="n">
+        <v>72.9750515095016</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.422234743611106</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
         <v>0.0651955322211558</v>
       </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
         <v>0.820274578370308</v>
       </c>
-      <c r="G24" t="n">
+      <c r="J24" t="n">
         <v>0.885470110591464</v>
       </c>
-      <c r="H24" t="n">
+      <c r="K24" t="n">
         <v>0.0525607762139513</v>
       </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C25" t="n">
         <v>696.579241968791</v>
@@ -1195,30 +1420,39 @@
         <v>50.4028055866973</v>
       </c>
       <c r="E25" t="n">
+        <v>50.4028055866973</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
         <v>1.00731407275454</v>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
         <v>2.17548736413844</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
         <v>3.18280143689298</v>
       </c>
-      <c r="H25" t="n">
+      <c r="K25" t="n">
         <v>0.0499390781770046</v>
       </c>
-      <c r="I25" t="n">
+      <c r="L25" t="n">
         <v>6.91275271931642</v>
       </c>
-      <c r="J25" t="n">
+      <c r="M25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C26" t="n">
         <v>360.445295876547</v>
@@ -1227,21 +1461,30 @@
         <v>49.3626292399363</v>
       </c>
       <c r="E26" t="n">
+        <v>50.0073633151328</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.644734075196555</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
         <v>0.0651955322211558</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>1.64054915674062</v>
       </c>
-      <c r="G26" t="n">
+      <c r="J26" t="n">
         <v>1.70574468896178</v>
       </c>
-      <c r="H26" t="n">
+      <c r="K26" t="n">
         <v>0.0534003963331417</v>
       </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>